<commit_message>
upadte prompt and add multi threads
</commit_message>
<xml_diff>
--- a/base_produtos_financeiros.xlsx
+++ b/base_produtos_financeiros.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="332">
   <si>
     <t>Produtos Financeiros</t>
   </si>
@@ -533,6 +533,483 @@
   </si>
   <si>
     <t>Renda+ Aposentadoria Extra 2065</t>
+  </si>
+  <si>
+    <t>LCA ABC</t>
+  </si>
+  <si>
+    <t>11,4% a.a.</t>
+  </si>
+  <si>
+    <t>95% do CDI</t>
+  </si>
+  <si>
+    <t>LCA ABC LIQUIDEZ</t>
+  </si>
+  <si>
+    <t>86% do CDI</t>
+  </si>
+  <si>
+    <t>LCA BDMG</t>
+  </si>
+  <si>
+    <t>94% do CDI</t>
+  </si>
+  <si>
+    <t>LCA BDMG LIQUIDEZ</t>
+  </si>
+  <si>
+    <t>LCA BOCOM</t>
+  </si>
+  <si>
+    <t>IPCA + 5% a.a.</t>
+  </si>
+  <si>
+    <t>IPCA + 5,1% a.a.</t>
+  </si>
+  <si>
+    <t>IPCA + 5,8% a.a.</t>
+  </si>
+  <si>
+    <t>10% a.a.</t>
+  </si>
+  <si>
+    <t>IPCA + 5,2% a.a.</t>
+  </si>
+  <si>
+    <t>IPCA + 5,5% a.a.</t>
+  </si>
+  <si>
+    <t>LCA BRB LIQUIDEZ</t>
+  </si>
+  <si>
+    <t>LCA BANCO VOTORANTIM S.A.</t>
+  </si>
+  <si>
+    <t>10,2% a.a.</t>
+  </si>
+  <si>
+    <t>10,3% a.a.</t>
+  </si>
+  <si>
+    <t>10,4% a.a.</t>
+  </si>
+  <si>
+    <t>10,8% a.a.</t>
+  </si>
+  <si>
+    <t>LIG Inter</t>
+  </si>
+  <si>
+    <t>LCI</t>
+  </si>
+  <si>
+    <t>87% do CDI</t>
+  </si>
+  <si>
+    <t>TPF - TÍTULO PÚBLICO</t>
+  </si>
+  <si>
+    <t>IPCA + 5,7% a.a.</t>
+  </si>
+  <si>
+    <t>CDB INTER LIQUIDEZ DIARIA</t>
+  </si>
+  <si>
+    <t>Até 102% do CDI</t>
+  </si>
+  <si>
+    <t>CDB MERCANTIL LIQUIDEZ - 101% do CDI</t>
+  </si>
+  <si>
+    <t>101% do CDI</t>
+  </si>
+  <si>
+    <t>LCI BRB LIQUIDEZ - 86% do CDI</t>
+  </si>
+  <si>
+    <t>LCA ABC LIQUIDEZ - 86% do CDI</t>
+  </si>
+  <si>
+    <t>LIG LIQUIDEZ - 87% do CDI</t>
+  </si>
+  <si>
+    <t>LCI DI LIQUIDEZ 9 MESES</t>
+  </si>
+  <si>
+    <t>Até 96% do CDI</t>
+  </si>
+  <si>
+    <t>CRI PATRIMAR E121 S1 - CDI + 1,7% a.a.</t>
+  </si>
+  <si>
+    <t>CRI</t>
+  </si>
+  <si>
+    <t>CDI + 1,7% a.a.</t>
+  </si>
+  <si>
+    <t>CRA AGRO SÃO JOSÉ E170 S1 - CDI + 3% a.a.</t>
+  </si>
+  <si>
+    <t>CRA</t>
+  </si>
+  <si>
+    <t>CDI + 3% a.a.</t>
+  </si>
+  <si>
+    <t>CRA CERRADÃO E162 S1 - IPCA + 7,75% a.a.</t>
+  </si>
+  <si>
+    <t>IPCA + 7,75% a.a.</t>
+  </si>
+  <si>
+    <t>CDB AFINZ - 117% do CDI</t>
+  </si>
+  <si>
+    <t>117% do CDI</t>
+  </si>
+  <si>
+    <t>CDB AFINZ - 112% do CDI</t>
+  </si>
+  <si>
+    <t>112% do CDI</t>
+  </si>
+  <si>
+    <t>CDB AFINZ - 119% do CDI</t>
+  </si>
+  <si>
+    <t>119% do CDI</t>
+  </si>
+  <si>
+    <t>CDB DIGIMAIS - 102% do CDI</t>
+  </si>
+  <si>
+    <t>102% do CDI</t>
+  </si>
+  <si>
+    <t>CDB DIGIMAIS - 109% do CDI</t>
+  </si>
+  <si>
+    <t>109% do CDI</t>
+  </si>
+  <si>
+    <t>CDB DIGIMAIS - 112% do CDI</t>
+  </si>
+  <si>
+    <t>CDB DIGIMAIS - 113% do CDI</t>
+  </si>
+  <si>
+    <t>113% do CDI</t>
+  </si>
+  <si>
+    <t>CDB GUANABARA - 99% do CDI</t>
+  </si>
+  <si>
+    <t>99% do CDI</t>
+  </si>
+  <si>
+    <t>CDB GUANABARA - 107% do CDI</t>
+  </si>
+  <si>
+    <t>107% do CDI</t>
+  </si>
+  <si>
+    <t>CDB GUANABARA - 108% do CDI</t>
+  </si>
+  <si>
+    <t>108% do CDI</t>
+  </si>
+  <si>
+    <t>CDB GUANABARA - 110% do CDI</t>
+  </si>
+  <si>
+    <t>110% do CDI</t>
+  </si>
+  <si>
+    <t>CDB GUANABARA - 111% do CDI</t>
+  </si>
+  <si>
+    <t>111% do CDI</t>
+  </si>
+  <si>
+    <t>CDB LETSBANK - 13,7% a.a.</t>
+  </si>
+  <si>
+    <t>13,7% a.a.</t>
+  </si>
+  <si>
+    <t>CDB MERCADO LIVRE - 99,5% do CDI</t>
+  </si>
+  <si>
+    <t>99,5% do CDI</t>
+  </si>
+  <si>
+    <t>CDB MERCADO LIVRE - 99,8% do CDI</t>
+  </si>
+  <si>
+    <t>99,8% do CDI</t>
+  </si>
+  <si>
+    <t>CDB MERCADO LIVRE - 100% do CDI</t>
+  </si>
+  <si>
+    <t>100% do CDI</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA - CRA LAR COOP E120 S1</t>
+  </si>
+  <si>
+    <t>IPCA + 6,9% a.a.</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA - CRA LOCALIZA E104 S1</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA - CRA LOCALIZA E157 S1</t>
+  </si>
+  <si>
+    <t>IPCA + 6,65% a.a.</t>
+  </si>
+  <si>
+    <t>ISEC Securitizadora - CRA M. DIAS BRANCO E25 S2</t>
+  </si>
+  <si>
+    <t>IPCA + 6,3% a.a.</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA - CRA MADERO E141 S1</t>
+  </si>
+  <si>
+    <t>IPCA + 7,1% a.a.</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA - CRA MARFRIG E153 S2</t>
+  </si>
+  <si>
+    <t>IPCA + 6,7% a.a.</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA - CRA MARFRIG E153 S3</t>
+  </si>
+  <si>
+    <t>IPCA + 6,85% a.a.</t>
+  </si>
+  <si>
+    <t>OPEA Securitizadora - CRA MARFRIG E16 S2</t>
+  </si>
+  <si>
+    <t>IPCA + 7% a.a.</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA - CRA MARFRIG E219 S1</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA - CRA MARFRIG E273 S1</t>
+  </si>
+  <si>
+    <t>11,7% a.a.</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA - CRA MARFRIG E273 S3</t>
+  </si>
+  <si>
+    <t>IPCA + 6,8% a.a.</t>
+  </si>
+  <si>
+    <t>VIRGO Companhia - CRA MINERVA E179 S2</t>
+  </si>
+  <si>
+    <t>12,3% a.a.</t>
+  </si>
+  <si>
+    <t>VIRGO Companhia - CRA MINERVA E179 S4</t>
+  </si>
+  <si>
+    <t>VIRGO Companhia - CRA MINERVA E39 S1</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA DE DIREITOS CREDITÓRIOS DO AGRONEGÓCIO S/A - CRA SOROCABA (COCA-COLA) E342 S2</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA DE DIREITOS CREDITÓRIOS DO AGRONEGÓCIO S/A - CRA TEDESCO E301 S1</t>
+  </si>
+  <si>
+    <t>CDI + 5,5% a.a.</t>
+  </si>
+  <si>
+    <t>VERT COMPANHIA SECURITIZADORA - CRA TEREOS E52 S1</t>
+  </si>
+  <si>
+    <t>IPCA + 6,5% a.a.</t>
+  </si>
+  <si>
+    <t>OPEA SECURITIZADORA S/A - CRA UNIDAS E121 S2</t>
+  </si>
+  <si>
+    <t>12,65% a.a.</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA DE DIREITOS CREDITÓRIOS DO AGRONEGÓCIO S/A - CRA VALE DO TIJUCO E128 S1</t>
+  </si>
+  <si>
+    <t>IPCA + 7,4% a.a.</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA DE DIREITOS CREDITÓRIOS DO AGRONEGÓCIO S/A - CRA VAMOS E23 S2</t>
+  </si>
+  <si>
+    <t>11% a.a.</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA DE DIREITOS CREDITÓRIOS DO AGRONEGÓCIO S/A - CRA VAMOS E296 S1</t>
+  </si>
+  <si>
+    <t>12,35% a.a.</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA DE DIREITOS CREDITÓRIOS DO AGRONEGÓCIO S/A - CRA VAMOS E296 S2</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA DE DIREITOS CREDITÓRIOS DO AGRONEGÓCIO S/A - CRA VAMOS E296 S3</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA S/A - CRA VAMOS E54 S1</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA S/A - CRA VAMOS E81 S1</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA DE DIREITOS CREDITÓRIOS DO AGRONEGÓCIO S/A - CRA VAMOS E93 S1</t>
+  </si>
+  <si>
+    <t>ECO SECURITIZADORA DE DIREITOS CREDITÓRIOS DO AGRONEGÓCIO S/A - CRA VAMOS E93 S2</t>
+  </si>
+  <si>
+    <t>VIRGO COMPANHIA DE SECURITIZAÇÃO - CRA VICUNHA E123 S1</t>
+  </si>
+  <si>
+    <t>VIRGO COMPANHIA DE SECURITIZAÇÃO - CRA VICUNHA E123 S2</t>
+  </si>
+  <si>
+    <t>CDI + 1,05% a.a.</t>
+  </si>
+  <si>
+    <t>VIRGO COMPANHIA DE SECURITIZAÇÃO - CRA VICUNHA E186 S1</t>
+  </si>
+  <si>
+    <t>CDI + 1,55% a.a.</t>
+  </si>
+  <si>
+    <t>VIRGO COMPANHIA DE SECURITIZAÇÃO - CRA VICUNHA E186 S2</t>
+  </si>
+  <si>
+    <t>12,8% a.a.</t>
+  </si>
+  <si>
+    <t>VIRGO COMPANHIA DE SECURITIZAÇÃO - CRA VICUNHA E186 S3</t>
+  </si>
+  <si>
+    <t>IPCA + 7,7% a.a.</t>
+  </si>
+  <si>
+    <t>TRUE SECURITIZADORA S/A - CRA ZILOR E16 S1</t>
+  </si>
+  <si>
+    <t>3R PETROLEUM ÓLEO E GÁS S/A - DEB 3R</t>
+  </si>
+  <si>
+    <t>DEB</t>
+  </si>
+  <si>
+    <t>IPCA + 7,3% a.a.</t>
+  </si>
+  <si>
+    <t>AES CAJUÍNA AB1 HOLDINGS S/A - DEB AES CAJUÍNA</t>
+  </si>
+  <si>
+    <t>AES TIETÊ ENERGIA S/A - DEB AES TIETÊ</t>
+  </si>
+  <si>
+    <t>Arteris S/A</t>
+  </si>
+  <si>
+    <t>Brisanet Serviços de Telecomunicações S/A</t>
+  </si>
+  <si>
+    <t>IPCA + 6,55% a.a.</t>
+  </si>
+  <si>
+    <t>Companhia de Água e Esgoto do Ceará (CAGECE)</t>
+  </si>
+  <si>
+    <t>IPCA + 6,95% a.a.</t>
+  </si>
+  <si>
+    <t>CCR S/A</t>
+  </si>
+  <si>
+    <t>IPCA + 5,9% a.a.</t>
+  </si>
+  <si>
+    <t>Cemig Distribuição S/A</t>
+  </si>
+  <si>
+    <t>IPCA + 6,25% a.a.</t>
+  </si>
+  <si>
+    <t>Companhia Hidroelétrica do São Francisco (CHESF)</t>
+  </si>
+  <si>
+    <t>IPCA + 6,4% a.a.</t>
+  </si>
+  <si>
+    <t>Ciclus Ambiental do Brasil S/A</t>
+  </si>
+  <si>
+    <t>Colombo Agroindústria S/A</t>
+  </si>
+  <si>
+    <t>Copel Distribuição S/A</t>
+  </si>
+  <si>
+    <t>IPCA + 6,15% a.a.</t>
+  </si>
+  <si>
+    <t>Companhia Siderúrgica Nacional</t>
+  </si>
+  <si>
+    <t>CSN Mineração S/A</t>
+  </si>
+  <si>
+    <t>IPCA + 6,75% a.a.</t>
+  </si>
+  <si>
+    <t>Ecorodovias Concessões e Serviços S/A</t>
+  </si>
+  <si>
+    <t>Centrais Elétricas Brasileiras S/A</t>
+  </si>
+  <si>
+    <t>Centrais Elétricas do Norte do Brasil S/A - Eletronorte</t>
+  </si>
+  <si>
+    <t>Enauta Participações S/A</t>
+  </si>
+  <si>
+    <t>13% a.a.</t>
+  </si>
+  <si>
+    <t>IPCA + 7,15% a.a.</t>
+  </si>
+  <si>
+    <t>Eletropaulo Metropolitano Eletr. de SP S/A</t>
+  </si>
+  <si>
+    <t>Energisa S/A</t>
+  </si>
+  <si>
+    <t>Sofisa</t>
   </si>
 </sst>
 </file>
@@ -540,7 +1017,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -558,6 +1035,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -636,17 +1119,17 @@
     <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -3557,12 +4040,24 @@
       <c r="L99" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="14.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
-      <c r="C100" s="13"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="11"/>
+      <c r="A100" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" s="13">
+        <v>46289</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E100" s="14">
+        <v>10</v>
+      </c>
+      <c r="F100" s="11">
+        <v>1000.43</v>
+      </c>
       <c r="G100" s="5"/>
       <c r="H100" s="11"/>
       <c r="I100" s="11"/>
@@ -3571,12 +4066,24 @@
       <c r="L100" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="14.25">
-      <c r="A101" s="5"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="13"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="11"/>
+      <c r="A101" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" s="13">
+        <v>46594</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E101" s="14">
+        <v>10</v>
+      </c>
+      <c r="F101" s="11">
+        <v>1015.51</v>
+      </c>
       <c r="G101" s="5"/>
       <c r="H101" s="11"/>
       <c r="I101" s="11"/>
@@ -3585,12 +4092,24 @@
       <c r="L101" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="14.25">
-      <c r="A102" s="5"/>
-      <c r="B102" s="5"/>
-      <c r="C102" s="13"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="11"/>
+      <c r="A102" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="13">
+        <v>45779</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E102" s="14">
+        <v>10</v>
+      </c>
+      <c r="F102" s="11">
+        <v>105.33</v>
+      </c>
       <c r="G102" s="5"/>
       <c r="H102" s="11"/>
       <c r="I102" s="11"/>
@@ -3599,12 +4118,24 @@
       <c r="L102" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="14.25">
-      <c r="A103" s="5"/>
-      <c r="B103" s="5"/>
-      <c r="C103" s="13"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="11"/>
+      <c r="A103" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="13">
+        <v>46462</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E103" s="14">
+        <v>10</v>
+      </c>
+      <c r="F103" s="11">
+        <v>1005.65</v>
+      </c>
       <c r="G103" s="5"/>
       <c r="H103" s="11"/>
       <c r="I103" s="11"/>
@@ -3613,12 +4144,24 @@
       <c r="L103" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="14.25">
-      <c r="A104" s="5"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="13"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="14"/>
-      <c r="F104" s="11"/>
+      <c r="A104" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="13">
+        <v>45901</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E104" s="14">
+        <v>61</v>
+      </c>
+      <c r="F104" s="11">
+        <v>101.34</v>
+      </c>
       <c r="G104" s="5"/>
       <c r="H104" s="11"/>
       <c r="I104" s="11"/>
@@ -3627,12 +4170,24 @@
       <c r="L104" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="14.25">
-      <c r="A105" s="5"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="13"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="11"/>
+      <c r="A105" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" s="13">
+        <v>46237</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E105" s="14">
+        <v>2</v>
+      </c>
+      <c r="F105" s="11">
+        <v>1015.02</v>
+      </c>
       <c r="G105" s="5"/>
       <c r="H105" s="11"/>
       <c r="I105" s="11"/>
@@ -3641,12 +4196,24 @@
       <c r="L105" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="14.25">
-      <c r="A106" s="5"/>
-      <c r="B106" s="5"/>
-      <c r="C106" s="13"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="11"/>
+      <c r="A106" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" s="13">
+        <v>46247</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E106" s="14">
+        <v>2</v>
+      </c>
+      <c r="F106" s="11">
+        <v>1009.48</v>
+      </c>
       <c r="G106" s="5"/>
       <c r="H106" s="11"/>
       <c r="I106" s="11"/>
@@ -3655,12 +4222,24 @@
       <c r="L106" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="14.25">
-      <c r="A107" s="5"/>
-      <c r="B107" s="5"/>
-      <c r="C107" s="13"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="14"/>
-      <c r="F107" s="11"/>
+      <c r="A107" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107" s="13">
+        <v>46295</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E107" s="14">
+        <v>2</v>
+      </c>
+      <c r="F107" s="11">
+        <v>1002.16</v>
+      </c>
       <c r="G107" s="5"/>
       <c r="H107" s="11"/>
       <c r="I107" s="11"/>
@@ -3669,12 +4248,24 @@
       <c r="L107" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="14.25">
-      <c r="A108" s="5"/>
-      <c r="B108" s="5"/>
-      <c r="C108" s="13"/>
-      <c r="D108" s="5"/>
-      <c r="E108" s="14"/>
-      <c r="F108" s="11"/>
+      <c r="A108" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" s="13">
+        <v>46524</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E108" s="14">
+        <v>2</v>
+      </c>
+      <c r="F108" s="11">
+        <v>1047.82</v>
+      </c>
       <c r="G108" s="5"/>
       <c r="H108" s="11"/>
       <c r="I108" s="11"/>
@@ -3683,12 +4274,24 @@
       <c r="L108" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="14.25">
-      <c r="A109" s="5"/>
-      <c r="B109" s="5"/>
-      <c r="C109" s="13"/>
-      <c r="D109" s="5"/>
-      <c r="E109" s="14"/>
-      <c r="F109" s="11"/>
+      <c r="A109" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" s="13">
+        <v>46640</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E109" s="14">
+        <v>2</v>
+      </c>
+      <c r="F109" s="11">
+        <v>1004.04</v>
+      </c>
       <c r="G109" s="5"/>
       <c r="H109" s="11"/>
       <c r="I109" s="11"/>
@@ -3697,12 +4300,24 @@
       <c r="L109" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="14.25">
-      <c r="A110" s="5"/>
-      <c r="B110" s="5"/>
-      <c r="C110" s="13"/>
-      <c r="D110" s="5"/>
-      <c r="E110" s="14"/>
-      <c r="F110" s="11"/>
+      <c r="A110" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" s="13">
+        <v>46650</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E110" s="14">
+        <v>2</v>
+      </c>
+      <c r="F110" s="11">
+        <v>1005.16</v>
+      </c>
       <c r="G110" s="5"/>
       <c r="H110" s="11"/>
       <c r="I110" s="11"/>
@@ -3711,12 +4326,24 @@
       <c r="L110" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="14.25">
-      <c r="A111" s="5"/>
-      <c r="B111" s="5"/>
-      <c r="C111" s="13"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="14"/>
-      <c r="F111" s="11"/>
+      <c r="A111" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" s="13">
+        <v>45793</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E111" s="14">
+        <v>5</v>
+      </c>
+      <c r="F111" s="11">
+        <v>102.13</v>
+      </c>
       <c r="G111" s="5"/>
       <c r="H111" s="11"/>
       <c r="I111" s="11"/>
@@ -3725,12 +4352,24 @@
       <c r="L111" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="14.25">
-      <c r="A112" s="5"/>
-      <c r="B112" s="5"/>
-      <c r="C112" s="13"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="11"/>
+      <c r="A112" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" s="13">
+        <v>45918</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E112" s="14">
+        <v>1</v>
+      </c>
+      <c r="F112" s="11">
+        <v>1005.29</v>
+      </c>
       <c r="G112" s="5"/>
       <c r="H112" s="11"/>
       <c r="I112" s="11"/>
@@ -3739,12 +4378,24 @@
       <c r="L112" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="14.25">
-      <c r="A113" s="5"/>
-      <c r="B113" s="5"/>
-      <c r="C113" s="13"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="11"/>
+      <c r="A113" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" s="13">
+        <v>45930</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E113" s="14">
+        <v>1</v>
+      </c>
+      <c r="F113" s="11">
+        <v>1002.05</v>
+      </c>
       <c r="G113" s="5"/>
       <c r="H113" s="11"/>
       <c r="I113" s="11"/>
@@ -3753,12 +4404,24 @@
       <c r="L113" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="14.25">
-      <c r="A114" s="5"/>
-      <c r="B114" s="5"/>
-      <c r="C114" s="13"/>
-      <c r="D114" s="5"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="11"/>
+      <c r="A114" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" s="13">
+        <v>46251</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E114" s="14">
+        <v>1</v>
+      </c>
+      <c r="F114" s="11">
+        <v>1014.36</v>
+      </c>
       <c r="G114" s="5"/>
       <c r="H114" s="11"/>
       <c r="I114" s="11"/>
@@ -3767,12 +4430,24 @@
       <c r="L114" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="14.25">
-      <c r="A115" s="5"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="13"/>
-      <c r="D115" s="5"/>
-      <c r="E115" s="14"/>
-      <c r="F115" s="11"/>
+      <c r="A115" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" s="13">
+        <v>46615</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E115" s="14">
+        <v>1</v>
+      </c>
+      <c r="F115" s="11">
+        <v>1014.1</v>
+      </c>
       <c r="G115" s="5"/>
       <c r="H115" s="11"/>
       <c r="I115" s="11"/>
@@ -3781,12 +4456,24 @@
       <c r="L115" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="14.25">
-      <c r="A116" s="5"/>
-      <c r="B116" s="5"/>
-      <c r="C116" s="13"/>
-      <c r="D116" s="5"/>
-      <c r="E116" s="14"/>
-      <c r="F116" s="11"/>
+      <c r="A116" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" s="13">
+        <v>46622</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E116" s="14">
+        <v>1</v>
+      </c>
+      <c r="F116" s="11">
+        <v>1012.64</v>
+      </c>
       <c r="G116" s="5"/>
       <c r="H116" s="11"/>
       <c r="I116" s="11"/>
@@ -3795,12 +4482,24 @@
       <c r="L116" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="14.25">
-      <c r="A117" s="5"/>
-      <c r="B117" s="5"/>
-      <c r="C117" s="13"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="14"/>
-      <c r="F117" s="11"/>
+      <c r="A117" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C117" s="13">
+        <v>46632</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E117" s="14">
+        <v>1</v>
+      </c>
+      <c r="F117" s="11">
+        <v>1005.35</v>
+      </c>
       <c r="G117" s="5"/>
       <c r="H117" s="11"/>
       <c r="I117" s="11"/>
@@ -3809,12 +4508,24 @@
       <c r="L117" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="14.25">
-      <c r="A118" s="5"/>
-      <c r="B118" s="5"/>
-      <c r="C118" s="13"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="14"/>
-      <c r="F118" s="11"/>
+      <c r="A118" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C118" s="13">
+        <v>46643</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E118" s="14">
+        <v>1</v>
+      </c>
+      <c r="F118" s="11">
+        <v>100464.17</v>
+      </c>
       <c r="G118" s="5"/>
       <c r="H118" s="11"/>
       <c r="I118" s="11"/>
@@ -3823,12 +4534,24 @@
       <c r="L118" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="14.25">
-      <c r="A119" s="5"/>
-      <c r="B119" s="5"/>
-      <c r="C119" s="13"/>
-      <c r="D119" s="5"/>
-      <c r="E119" s="14"/>
-      <c r="F119" s="11"/>
+      <c r="A119" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C119" s="13">
+        <v>46625</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E119" s="14">
+        <v>1</v>
+      </c>
+      <c r="F119" s="11">
+        <v>1004.59</v>
+      </c>
       <c r="G119" s="5"/>
       <c r="H119" s="11"/>
       <c r="I119" s="11"/>
@@ -3837,12 +4560,24 @@
       <c r="L119" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="14.25">
-      <c r="A120" s="5"/>
-      <c r="B120" s="5"/>
-      <c r="C120" s="13"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="14"/>
-      <c r="F120" s="11"/>
+      <c r="A120" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C120" s="13">
+        <v>53097</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E120" s="14">
+        <v>20</v>
+      </c>
+      <c r="F120" s="11">
+        <v>4601.73</v>
+      </c>
       <c r="G120" s="5"/>
       <c r="H120" s="11"/>
       <c r="I120" s="11"/>
@@ -3851,12 +4586,24 @@
       <c r="L120" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="14.25">
-      <c r="A121" s="5"/>
-      <c r="B121" s="5"/>
-      <c r="C121" s="13"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="14"/>
-      <c r="F121" s="11"/>
+      <c r="A121" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C121" s="13">
+        <v>46813</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E121" s="14">
+        <v>5</v>
+      </c>
+      <c r="F121" s="11">
+        <v>15415.49</v>
+      </c>
       <c r="G121" s="5"/>
       <c r="H121" s="11"/>
       <c r="I121" s="11"/>
@@ -3865,12 +4612,24 @@
       <c r="L121" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="14.25">
-      <c r="A122" s="5"/>
-      <c r="B122" s="5"/>
-      <c r="C122" s="13"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="14"/>
-      <c r="F122" s="11"/>
+      <c r="A122" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C122" s="13">
+        <v>46291</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E122" s="14">
+        <v>1</v>
+      </c>
+      <c r="F122" s="11">
+        <v>1</v>
+      </c>
       <c r="G122" s="5"/>
       <c r="H122" s="11"/>
       <c r="I122" s="11"/>
@@ -3879,12 +4638,24 @@
       <c r="L122" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="14.25">
-      <c r="A123" s="5"/>
-      <c r="B123" s="5"/>
-      <c r="C123" s="13"/>
-      <c r="D123" s="5"/>
-      <c r="E123" s="14"/>
-      <c r="F123" s="11"/>
+      <c r="A123" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C123" s="13">
+        <v>45919</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E123" s="14">
+        <v>1</v>
+      </c>
+      <c r="F123" s="11">
+        <v>100.43</v>
+      </c>
       <c r="G123" s="5"/>
       <c r="H123" s="11"/>
       <c r="I123" s="11"/>
@@ -3893,12 +4664,24 @@
       <c r="L123" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="14.25">
-      <c r="A124" s="5"/>
-      <c r="B124" s="5"/>
-      <c r="C124" s="13"/>
-      <c r="D124" s="5"/>
-      <c r="E124" s="14"/>
-      <c r="F124" s="11"/>
+      <c r="A124" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C124" s="13">
+        <v>45761</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E124" s="14">
+        <v>1</v>
+      </c>
+      <c r="F124" s="11">
+        <v>105.66</v>
+      </c>
       <c r="G124" s="5"/>
       <c r="H124" s="11"/>
       <c r="I124" s="11"/>
@@ -3907,12 +4690,24 @@
       <c r="L124" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="14.25">
-      <c r="A125" s="5"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="13"/>
-      <c r="D125" s="5"/>
-      <c r="E125" s="14"/>
-      <c r="F125" s="11"/>
+      <c r="A125" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" s="13">
+        <v>45842</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E125" s="14">
+        <v>2</v>
+      </c>
+      <c r="F125" s="11">
+        <v>103.3</v>
+      </c>
       <c r="G125" s="5"/>
       <c r="H125" s="11"/>
       <c r="I125" s="11"/>
@@ -3921,12 +4716,24 @@
       <c r="L125" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="14.25">
-      <c r="A126" s="5"/>
-      <c r="B126" s="5"/>
-      <c r="C126" s="13"/>
-      <c r="D126" s="5"/>
-      <c r="E126" s="14"/>
-      <c r="F126" s="11"/>
+      <c r="A126" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C126" s="13">
+        <v>46636</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E126" s="14">
+        <v>5</v>
+      </c>
+      <c r="F126" s="11">
+        <v>99.42</v>
+      </c>
       <c r="G126" s="5"/>
       <c r="H126" s="11"/>
       <c r="I126" s="11"/>
@@ -3935,12 +4742,24 @@
       <c r="L126" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="14.25">
-      <c r="A127" s="5"/>
-      <c r="B127" s="5"/>
-      <c r="C127" s="13"/>
-      <c r="D127" s="5"/>
-      <c r="E127" s="14"/>
-      <c r="F127" s="11"/>
+      <c r="A127" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C127" s="13">
+        <v>46651</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E127" s="14">
+        <v>2</v>
+      </c>
+      <c r="F127" s="11">
+        <v>50</v>
+      </c>
       <c r="G127" s="5"/>
       <c r="H127" s="11"/>
       <c r="I127" s="11"/>
@@ -3949,12 +4768,24 @@
       <c r="L127" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="14.25">
-      <c r="A128" s="5"/>
-      <c r="B128" s="5"/>
-      <c r="C128" s="13"/>
-      <c r="D128" s="5"/>
-      <c r="E128" s="14"/>
-      <c r="F128" s="11"/>
+      <c r="A128" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C128" s="13">
+        <v>47046</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E128" s="14">
+        <v>20</v>
+      </c>
+      <c r="F128" s="11">
+        <v>1064.9</v>
+      </c>
       <c r="G128" s="5"/>
       <c r="H128" s="11"/>
       <c r="I128" s="11"/>
@@ -3963,12 +4794,24 @@
       <c r="L128" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="14.25">
-      <c r="A129" s="5"/>
-      <c r="B129" s="5"/>
-      <c r="C129" s="13"/>
-      <c r="D129" s="5"/>
-      <c r="E129" s="14"/>
-      <c r="F129" s="11"/>
+      <c r="A129" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C129" s="13">
+        <v>46763</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E129" s="14">
+        <v>20</v>
+      </c>
+      <c r="F129" s="11">
+        <v>972.71</v>
+      </c>
       <c r="G129" s="5"/>
       <c r="H129" s="11"/>
       <c r="I129" s="11"/>
@@ -3977,12 +4820,24 @@
       <c r="L129" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="14.25">
-      <c r="A130" s="5"/>
-      <c r="B130" s="5"/>
-      <c r="C130" s="13"/>
-      <c r="D130" s="5"/>
-      <c r="E130" s="14"/>
-      <c r="F130" s="11"/>
+      <c r="A130" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C130" s="13">
+        <v>46888</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E130" s="14">
+        <v>20</v>
+      </c>
+      <c r="F130" s="11">
+        <v>1103.85</v>
+      </c>
       <c r="G130" s="5"/>
       <c r="H130" s="11"/>
       <c r="I130" s="11"/>
@@ -3991,12 +4846,24 @@
       <c r="L130" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="14.25">
-      <c r="A131" s="5"/>
-      <c r="B131" s="5"/>
-      <c r="C131" s="13"/>
-      <c r="D131" s="5"/>
-      <c r="E131" s="14"/>
-      <c r="F131" s="11"/>
+      <c r="A131" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C131" s="13">
+        <v>45754</v>
+      </c>
+      <c r="D131" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E131" s="14">
+        <v>10</v>
+      </c>
+      <c r="F131" s="11">
+        <v>1000</v>
+      </c>
       <c r="G131" s="5"/>
       <c r="H131" s="11"/>
       <c r="I131" s="11"/>
@@ -4005,12 +4872,24 @@
       <c r="L131" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="14.25">
-      <c r="A132" s="5"/>
-      <c r="B132" s="5"/>
-      <c r="C132" s="13"/>
-      <c r="D132" s="5"/>
-      <c r="E132" s="14"/>
-      <c r="F132" s="11"/>
+      <c r="A132" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C132" s="13">
+        <v>45939</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E132" s="14">
+        <v>10</v>
+      </c>
+      <c r="F132" s="11">
+        <v>1000</v>
+      </c>
       <c r="G132" s="5"/>
       <c r="H132" s="11"/>
       <c r="I132" s="11"/>
@@ -4019,12 +4898,24 @@
       <c r="L132" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="14.25">
-      <c r="A133" s="5"/>
-      <c r="B133" s="5"/>
-      <c r="C133" s="13"/>
-      <c r="D133" s="5"/>
-      <c r="E133" s="14"/>
-      <c r="F133" s="11"/>
+      <c r="A133" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C133" s="13">
+        <v>46114</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E133" s="14">
+        <v>10</v>
+      </c>
+      <c r="F133" s="11">
+        <v>1000</v>
+      </c>
       <c r="G133" s="5"/>
       <c r="H133" s="11"/>
       <c r="I133" s="11"/>
@@ -4033,12 +4924,24 @@
       <c r="L133" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="14.25">
-      <c r="A134" s="5"/>
-      <c r="B134" s="5"/>
-      <c r="C134" s="13"/>
-      <c r="D134" s="5"/>
-      <c r="E134" s="14"/>
-      <c r="F134" s="11"/>
+      <c r="A134" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C134" s="13">
+        <v>45939</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E134" s="14">
+        <v>2</v>
+      </c>
+      <c r="F134" s="11">
+        <v>5000</v>
+      </c>
       <c r="G134" s="5"/>
       <c r="H134" s="11"/>
       <c r="I134" s="11"/>
@@ -4047,12 +4950,24 @@
       <c r="L134" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="14.25">
-      <c r="A135" s="5"/>
-      <c r="B135" s="5"/>
-      <c r="C135" s="13"/>
-      <c r="D135" s="5"/>
-      <c r="E135" s="14"/>
-      <c r="F135" s="11"/>
+      <c r="A135" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C135" s="13">
+        <v>46293</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="E135" s="14">
+        <v>2</v>
+      </c>
+      <c r="F135" s="11">
+        <v>5000</v>
+      </c>
       <c r="G135" s="5"/>
       <c r="H135" s="11"/>
       <c r="I135" s="11"/>
@@ -4061,12 +4976,24 @@
       <c r="L135" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="14.25">
-      <c r="A136" s="5"/>
-      <c r="B136" s="5"/>
-      <c r="C136" s="13"/>
-      <c r="D136" s="5"/>
-      <c r="E136" s="14"/>
-      <c r="F136" s="11"/>
+      <c r="A136" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C136" s="13">
+        <v>46654</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E136" s="14">
+        <v>2</v>
+      </c>
+      <c r="F136" s="11">
+        <v>5000</v>
+      </c>
       <c r="G136" s="5"/>
       <c r="H136" s="11"/>
       <c r="I136" s="11"/>
@@ -4075,12 +5002,24 @@
       <c r="L136" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="14.25">
-      <c r="A137" s="5"/>
-      <c r="B137" s="5"/>
-      <c r="C137" s="13"/>
-      <c r="D137" s="5"/>
-      <c r="E137" s="14"/>
-      <c r="F137" s="11"/>
+      <c r="A137" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C137" s="13">
+        <v>47014</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E137" s="14">
+        <v>2</v>
+      </c>
+      <c r="F137" s="11">
+        <v>5000</v>
+      </c>
       <c r="G137" s="5"/>
       <c r="H137" s="11"/>
       <c r="I137" s="11"/>
@@ -4089,12 +5028,24 @@
       <c r="L137" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="14.25">
-      <c r="A138" s="5"/>
-      <c r="B138" s="5"/>
-      <c r="C138" s="13"/>
-      <c r="D138" s="5"/>
-      <c r="E138" s="14"/>
-      <c r="F138" s="11"/>
+      <c r="A138" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C138" s="13">
+        <v>47374</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E138" s="14">
+        <v>2</v>
+      </c>
+      <c r="F138" s="11">
+        <v>5000</v>
+      </c>
       <c r="G138" s="5"/>
       <c r="H138" s="11"/>
       <c r="I138" s="11"/>
@@ -4103,12 +5054,24 @@
       <c r="L138" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="14.25">
-      <c r="A139" s="5"/>
-      <c r="B139" s="5"/>
-      <c r="C139" s="13"/>
-      <c r="D139" s="5"/>
-      <c r="E139" s="14"/>
-      <c r="F139" s="11"/>
+      <c r="A139" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C139" s="13">
+        <v>47763</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E139" s="14">
+        <v>2</v>
+      </c>
+      <c r="F139" s="11">
+        <v>100</v>
+      </c>
       <c r="G139" s="5"/>
       <c r="H139" s="11"/>
       <c r="I139" s="11"/>
@@ -4117,12 +5080,24 @@
       <c r="L139" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="14.25">
-      <c r="A140" s="5"/>
-      <c r="B140" s="5"/>
-      <c r="C140" s="13"/>
-      <c r="D140" s="5"/>
-      <c r="E140" s="14"/>
-      <c r="F140" s="11"/>
+      <c r="A140" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C140" s="13">
+        <v>45754</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E140" s="14">
+        <v>10</v>
+      </c>
+      <c r="F140" s="11">
+        <v>1000</v>
+      </c>
       <c r="G140" s="5"/>
       <c r="H140" s="11"/>
       <c r="I140" s="11"/>
@@ -4131,12 +5106,24 @@
       <c r="L140" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="14.25">
-      <c r="A141" s="5"/>
-      <c r="B141" s="5"/>
-      <c r="C141" s="13"/>
-      <c r="D141" s="5"/>
-      <c r="E141" s="14"/>
-      <c r="F141" s="11"/>
+      <c r="A141" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C141" s="13">
+        <v>45933</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E141" s="14">
+        <v>10</v>
+      </c>
+      <c r="F141" s="11">
+        <v>1000</v>
+      </c>
       <c r="G141" s="5"/>
       <c r="H141" s="11"/>
       <c r="I141" s="11"/>
@@ -4145,12 +5132,24 @@
       <c r="L141" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="14.25">
-      <c r="A142" s="5"/>
-      <c r="B142" s="5"/>
-      <c r="C142" s="13"/>
-      <c r="D142" s="5"/>
-      <c r="E142" s="14"/>
-      <c r="F142" s="11"/>
+      <c r="A142" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C142" s="13">
+        <v>46293</v>
+      </c>
+      <c r="D142" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="E142" s="14">
+        <v>10</v>
+      </c>
+      <c r="F142" s="11">
+        <v>1000</v>
+      </c>
       <c r="G142" s="5"/>
       <c r="H142" s="11"/>
       <c r="I142" s="11"/>
@@ -4159,12 +5158,24 @@
       <c r="L142" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="14.25">
-      <c r="A143" s="5"/>
-      <c r="B143" s="5"/>
-      <c r="C143" s="13"/>
-      <c r="D143" s="5"/>
-      <c r="E143" s="14"/>
-      <c r="F143" s="11"/>
+      <c r="A143" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C143" s="13">
+        <v>46653</v>
+      </c>
+      <c r="D143" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E143" s="14">
+        <v>10</v>
+      </c>
+      <c r="F143" s="11">
+        <v>1000</v>
+      </c>
       <c r="G143" s="5"/>
       <c r="H143" s="11"/>
       <c r="I143" s="11"/>
@@ -4173,12 +5184,24 @@
       <c r="L143" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="14.25">
-      <c r="A144" s="5"/>
-      <c r="B144" s="5"/>
-      <c r="C144" s="13"/>
-      <c r="D144" s="5"/>
-      <c r="E144" s="14"/>
-      <c r="F144" s="11"/>
+      <c r="A144" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C144" s="13">
+        <v>47014</v>
+      </c>
+      <c r="D144" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E144" s="14">
+        <v>10</v>
+      </c>
+      <c r="F144" s="11">
+        <v>1000</v>
+      </c>
       <c r="G144" s="5"/>
       <c r="H144" s="11"/>
       <c r="I144" s="11"/>
@@ -4187,12 +5210,24 @@
       <c r="L144" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="14.25">
-      <c r="A145" s="5"/>
-      <c r="B145" s="5"/>
-      <c r="C145" s="13"/>
-      <c r="D145" s="5"/>
-      <c r="E145" s="14"/>
-      <c r="F145" s="11"/>
+      <c r="A145" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C145" s="13">
+        <v>47374</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E145" s="14">
+        <v>10</v>
+      </c>
+      <c r="F145" s="11">
+        <v>1000</v>
+      </c>
       <c r="G145" s="5"/>
       <c r="H145" s="11"/>
       <c r="I145" s="11"/>
@@ -4201,12 +5236,24 @@
       <c r="L145" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="14.25">
-      <c r="A146" s="5"/>
-      <c r="B146" s="5"/>
-      <c r="C146" s="13"/>
-      <c r="D146" s="5"/>
-      <c r="E146" s="14"/>
-      <c r="F146" s="11"/>
+      <c r="A146" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C146" s="13">
+        <v>45937</v>
+      </c>
+      <c r="D146" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E146" s="14">
+        <v>20</v>
+      </c>
+      <c r="F146" s="11">
+        <v>100</v>
+      </c>
       <c r="G146" s="5"/>
       <c r="H146" s="11"/>
       <c r="I146" s="11"/>
@@ -4215,12 +5262,24 @@
       <c r="L146" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="14.25">
-      <c r="A147" s="5"/>
-      <c r="B147" s="5"/>
-      <c r="C147" s="13"/>
-      <c r="D147" s="5"/>
-      <c r="E147" s="14"/>
-      <c r="F147" s="11"/>
+      <c r="A147" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C147" s="13">
+        <v>45663</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E147" s="14">
+        <v>20</v>
+      </c>
+      <c r="F147" s="11">
+        <v>1000</v>
+      </c>
       <c r="G147" s="5"/>
       <c r="H147" s="11"/>
       <c r="I147" s="11"/>
@@ -4229,12 +5288,24 @@
       <c r="L147" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="14.25">
-      <c r="A148" s="5"/>
-      <c r="B148" s="5"/>
-      <c r="C148" s="13"/>
-      <c r="D148" s="5"/>
-      <c r="E148" s="14"/>
-      <c r="F148" s="11"/>
+      <c r="A148" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C148" s="13">
+        <v>45754</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E148" s="14">
+        <v>20</v>
+      </c>
+      <c r="F148" s="11">
+        <v>1000</v>
+      </c>
       <c r="G148" s="5"/>
       <c r="H148" s="11"/>
       <c r="I148" s="11"/>
@@ -4243,12 +5314,24 @@
       <c r="L148" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="14.25">
-      <c r="A149" s="5"/>
-      <c r="B149" s="5"/>
-      <c r="C149" s="13"/>
-      <c r="D149" s="5"/>
-      <c r="E149" s="14"/>
-      <c r="F149" s="11"/>
+      <c r="A149" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C149" s="13">
+        <v>45932</v>
+      </c>
+      <c r="D149" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E149" s="14">
+        <v>20</v>
+      </c>
+      <c r="F149" s="11">
+        <v>1000</v>
+      </c>
       <c r="G149" s="5"/>
       <c r="H149" s="11"/>
       <c r="I149" s="11"/>
@@ -4257,12 +5340,24 @@
       <c r="L149" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="14.25">
-      <c r="A150" s="5"/>
-      <c r="B150" s="5"/>
-      <c r="C150" s="13"/>
-      <c r="D150" s="5"/>
-      <c r="E150" s="14"/>
-      <c r="F150" s="11"/>
+      <c r="A150" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C150" s="13">
+        <v>46341</v>
+      </c>
+      <c r="D150" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E150" s="14">
+        <v>40</v>
+      </c>
+      <c r="F150" s="11">
+        <v>1203.33</v>
+      </c>
       <c r="G150" s="5"/>
       <c r="H150" s="11"/>
       <c r="I150" s="11"/>
@@ -4271,12 +5366,24 @@
       <c r="L150" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="14.25">
-      <c r="A151" s="5"/>
-      <c r="B151" s="5"/>
-      <c r="C151" s="13"/>
-      <c r="D151" s="5"/>
-      <c r="E151" s="14"/>
-      <c r="F151" s="11"/>
+      <c r="A151" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C151" s="13">
+        <v>48044</v>
+      </c>
+      <c r="D151" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E151" s="14">
+        <v>40</v>
+      </c>
+      <c r="F151" s="11">
+        <v>1108.17</v>
+      </c>
       <c r="G151" s="5"/>
       <c r="H151" s="11"/>
       <c r="I151" s="11"/>
@@ -4285,12 +5392,24 @@
       <c r="L151" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="14.25">
-      <c r="A152" s="5"/>
-      <c r="B152" s="5"/>
-      <c r="C152" s="13"/>
-      <c r="D152" s="5"/>
-      <c r="E152" s="14"/>
-      <c r="F152" s="11"/>
+      <c r="A152" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C152" s="13">
+        <v>47011</v>
+      </c>
+      <c r="D152" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="E152" s="14">
+        <v>40</v>
+      </c>
+      <c r="F152" s="11">
+        <v>1097.64</v>
+      </c>
       <c r="G152" s="5"/>
       <c r="H152" s="11"/>
       <c r="I152" s="11"/>
@@ -4299,12 +5418,24 @@
       <c r="L152" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="14.25">
-      <c r="A153" s="5"/>
-      <c r="B153" s="5"/>
-      <c r="C153" s="13"/>
-      <c r="D153" s="5"/>
-      <c r="E153" s="14"/>
-      <c r="F153" s="11"/>
+      <c r="A153" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C153" s="13">
+        <v>47922</v>
+      </c>
+      <c r="D153" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E153" s="14">
+        <v>40</v>
+      </c>
+      <c r="F153" s="11">
+        <v>1130.84</v>
+      </c>
       <c r="G153" s="5"/>
       <c r="H153" s="11"/>
       <c r="I153" s="11"/>
@@ -4313,12 +5444,24 @@
       <c r="L153" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="14.25">
-      <c r="A154" s="5"/>
-      <c r="B154" s="5"/>
-      <c r="C154" s="13"/>
-      <c r="D154" s="5"/>
-      <c r="E154" s="14"/>
-      <c r="F154" s="11"/>
+      <c r="A154" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C154" s="13">
+        <v>46827</v>
+      </c>
+      <c r="D154" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E154" s="14">
+        <v>40</v>
+      </c>
+      <c r="F154" s="11">
+        <v>894.44</v>
+      </c>
       <c r="G154" s="5"/>
       <c r="H154" s="11"/>
       <c r="I154" s="11"/>
@@ -4327,12 +5470,24 @@
       <c r="L154" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="14.25">
-      <c r="A155" s="5"/>
-      <c r="B155" s="5"/>
-      <c r="C155" s="13"/>
-      <c r="D155" s="5"/>
-      <c r="E155" s="14"/>
-      <c r="F155" s="11"/>
+      <c r="A155" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C155" s="13">
+        <v>46402</v>
+      </c>
+      <c r="D155" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="E155" s="14">
+        <v>40</v>
+      </c>
+      <c r="F155" s="11">
+        <v>1145.35</v>
+      </c>
       <c r="G155" s="5"/>
       <c r="H155" s="11"/>
       <c r="I155" s="11"/>
@@ -4341,12 +5496,24 @@
       <c r="L155" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="14.25">
-      <c r="A156" s="5"/>
-      <c r="B156" s="5"/>
-      <c r="C156" s="13"/>
-      <c r="D156" s="5"/>
-      <c r="E156" s="14"/>
-      <c r="F156" s="11"/>
+      <c r="A156" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C156" s="13">
+        <v>48228</v>
+      </c>
+      <c r="D156" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E156" s="14">
+        <v>40</v>
+      </c>
+      <c r="F156" s="11">
+        <v>1145.55</v>
+      </c>
       <c r="G156" s="5"/>
       <c r="H156" s="11"/>
       <c r="I156" s="11"/>
@@ -4355,12 +5522,24 @@
       <c r="L156" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="14.25">
-      <c r="A157" s="5"/>
-      <c r="B157" s="5"/>
-      <c r="C157" s="13"/>
-      <c r="D157" s="5"/>
-      <c r="E157" s="14"/>
-      <c r="F157" s="11"/>
+      <c r="A157" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C157" s="13">
+        <v>48044</v>
+      </c>
+      <c r="D157" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E157" s="14">
+        <v>40</v>
+      </c>
+      <c r="F157" s="11">
+        <v>1084.87</v>
+      </c>
       <c r="G157" s="5"/>
       <c r="H157" s="11"/>
       <c r="I157" s="11"/>
@@ -4369,12 +5548,24 @@
       <c r="L157" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="14.25">
-      <c r="A158" s="5"/>
-      <c r="B158" s="5"/>
-      <c r="C158" s="13"/>
-      <c r="D158" s="5"/>
-      <c r="E158" s="14"/>
-      <c r="F158" s="11"/>
+      <c r="A158" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C158" s="13">
+        <v>47406</v>
+      </c>
+      <c r="D158" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="E158" s="14">
+        <v>40</v>
+      </c>
+      <c r="F158" s="11">
+        <v>1134.66</v>
+      </c>
       <c r="G158" s="5"/>
       <c r="H158" s="11"/>
       <c r="I158" s="11"/>
@@ -4383,12 +5574,24 @@
       <c r="L158" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="14.25">
-      <c r="A159" s="5"/>
-      <c r="B159" s="5"/>
-      <c r="C159" s="13"/>
-      <c r="D159" s="5"/>
-      <c r="E159" s="14"/>
-      <c r="F159" s="11"/>
+      <c r="A159" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B159" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C159" s="13">
+        <v>46615</v>
+      </c>
+      <c r="D159" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E159" s="14">
+        <v>35</v>
+      </c>
+      <c r="F159" s="11">
+        <v>999.71</v>
+      </c>
       <c r="G159" s="5"/>
       <c r="H159" s="11"/>
       <c r="I159" s="11"/>
@@ -4397,12 +5600,24 @@
       <c r="L159" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="14.25">
-      <c r="A160" s="5"/>
-      <c r="B160" s="5"/>
-      <c r="C160" s="13"/>
-      <c r="D160" s="5"/>
-      <c r="E160" s="14"/>
-      <c r="F160" s="11"/>
+      <c r="A160" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C160" s="13">
+        <v>47710</v>
+      </c>
+      <c r="D160" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="E160" s="14">
+        <v>40</v>
+      </c>
+      <c r="F160" s="11">
+        <v>1048.63</v>
+      </c>
       <c r="G160" s="5"/>
       <c r="H160" s="11"/>
       <c r="I160" s="11"/>
@@ -4411,12 +5626,24 @@
       <c r="L160" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="14.25">
-      <c r="A161" s="5"/>
-      <c r="B161" s="5"/>
-      <c r="C161" s="13"/>
-      <c r="D161" s="5"/>
-      <c r="E161" s="14"/>
-      <c r="F161" s="11"/>
+      <c r="A161" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C161" s="13">
+        <v>47011</v>
+      </c>
+      <c r="D161" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E161" s="14">
+        <v>30</v>
+      </c>
+      <c r="F161" s="11">
+        <v>1028.38</v>
+      </c>
       <c r="G161" s="5"/>
       <c r="H161" s="11"/>
       <c r="I161" s="11"/>
@@ -4425,12 +5652,24 @@
       <c r="L161" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="14.25">
-      <c r="A162" s="5"/>
-      <c r="B162" s="5"/>
-      <c r="C162" s="13"/>
-      <c r="D162" s="5"/>
-      <c r="E162" s="14"/>
-      <c r="F162" s="11"/>
+      <c r="A162" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C162" s="13">
+        <v>47742</v>
+      </c>
+      <c r="D162" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E162" s="14">
+        <v>30</v>
+      </c>
+      <c r="F162" s="11">
+        <v>1050.88</v>
+      </c>
       <c r="G162" s="5"/>
       <c r="H162" s="11"/>
       <c r="I162" s="11"/>
@@ -4439,12 +5678,24 @@
       <c r="L162" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="14.25">
-      <c r="A163" s="5"/>
-      <c r="B163" s="5"/>
-      <c r="C163" s="13"/>
-      <c r="D163" s="5"/>
-      <c r="E163" s="14"/>
-      <c r="F163" s="11"/>
+      <c r="A163" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C163" s="13">
+        <v>46860</v>
+      </c>
+      <c r="D163" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="E163" s="14">
+        <v>40</v>
+      </c>
+      <c r="F163" s="11">
+        <v>1216.41</v>
+      </c>
       <c r="G163" s="5"/>
       <c r="H163" s="11"/>
       <c r="I163" s="11"/>
@@ -4453,12 +5704,24 @@
       <c r="L163" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="14.25">
-      <c r="A164" s="5"/>
-      <c r="B164" s="5"/>
-      <c r="C164" s="13"/>
-      <c r="D164" s="5"/>
-      <c r="E164" s="14"/>
-      <c r="F164" s="11"/>
+      <c r="A164" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C164" s="13">
+        <v>49171</v>
+      </c>
+      <c r="D164" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E164" s="14">
+        <v>40</v>
+      </c>
+      <c r="F164" s="11">
+        <v>1007.38</v>
+      </c>
       <c r="G164" s="5"/>
       <c r="H164" s="11"/>
       <c r="I164" s="11"/>
@@ -4467,12 +5730,24 @@
       <c r="L164" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="14.25">
-      <c r="A165" s="5"/>
-      <c r="B165" s="5"/>
-      <c r="C165" s="13"/>
-      <c r="D165" s="5"/>
-      <c r="E165" s="14"/>
-      <c r="F165" s="11"/>
+      <c r="A165" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C165" s="13">
+        <v>48243</v>
+      </c>
+      <c r="D165" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E165" s="14">
+        <v>40</v>
+      </c>
+      <c r="F165" s="11">
+        <v>1045.2</v>
+      </c>
       <c r="G165" s="5"/>
       <c r="H165" s="11"/>
       <c r="I165" s="11"/>
@@ -4481,12 +5756,24 @@
       <c r="L165" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="14.25">
-      <c r="A166" s="5"/>
-      <c r="B166" s="5"/>
-      <c r="C166" s="13"/>
-      <c r="D166" s="5"/>
-      <c r="E166" s="14"/>
-      <c r="F166" s="11"/>
+      <c r="A166" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B166" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C166" s="13">
+        <v>46097</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="E166" s="14">
+        <v>40</v>
+      </c>
+      <c r="F166" s="11">
+        <v>827.96</v>
+      </c>
       <c r="G166" s="5"/>
       <c r="H166" s="11"/>
       <c r="I166" s="11"/>
@@ -4495,12 +5782,24 @@
       <c r="L166" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="14.25">
-      <c r="A167" s="5"/>
-      <c r="B167" s="5"/>
-      <c r="C167" s="13"/>
-      <c r="D167" s="5"/>
-      <c r="E167" s="14"/>
-      <c r="F167" s="11"/>
+      <c r="A167" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C167" s="13">
+        <v>47102</v>
+      </c>
+      <c r="D167" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="E167" s="14">
+        <v>40</v>
+      </c>
+      <c r="F167" s="11">
+        <v>1033.59</v>
+      </c>
       <c r="G167" s="5"/>
       <c r="H167" s="11"/>
       <c r="I167" s="11"/>
@@ -4509,12 +5808,24 @@
       <c r="L167" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="14.25">
-      <c r="A168" s="5"/>
-      <c r="B168" s="5"/>
-      <c r="C168" s="13"/>
-      <c r="D168" s="5"/>
-      <c r="E168" s="14"/>
-      <c r="F168" s="11"/>
+      <c r="A168" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C168" s="13">
+        <v>47133</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="E168" s="14">
+        <v>40</v>
+      </c>
+      <c r="F168" s="11">
+        <v>1120.61</v>
+      </c>
       <c r="G168" s="5"/>
       <c r="H168" s="11"/>
       <c r="I168" s="11"/>
@@ -4523,12 +5834,24 @@
       <c r="L168" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="14.25">
-      <c r="A169" s="5"/>
-      <c r="B169" s="5"/>
-      <c r="C169" s="13"/>
-      <c r="D169" s="5"/>
-      <c r="E169" s="14"/>
-      <c r="F169" s="11"/>
+      <c r="A169" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B169" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C169" s="13">
+        <v>46342</v>
+      </c>
+      <c r="D169" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E169" s="14">
+        <v>40</v>
+      </c>
+      <c r="F169" s="11">
+        <v>680.31</v>
+      </c>
       <c r="G169" s="5"/>
       <c r="H169" s="11"/>
       <c r="I169" s="11"/>
@@ -4537,12 +5860,24 @@
       <c r="L169" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="14.25">
-      <c r="A170" s="5"/>
-      <c r="B170" s="5"/>
-      <c r="C170" s="13"/>
-      <c r="D170" s="5"/>
-      <c r="E170" s="14"/>
-      <c r="F170" s="11"/>
+      <c r="A170" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C170" s="13">
+        <v>47805</v>
+      </c>
+      <c r="D170" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="E170" s="14">
+        <v>40</v>
+      </c>
+      <c r="F170" s="11">
+        <v>1035.15</v>
+      </c>
       <c r="G170" s="5"/>
       <c r="H170" s="11"/>
       <c r="I170" s="11"/>
@@ -4551,12 +5886,24 @@
       <c r="L170" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="14.25">
-      <c r="A171" s="5"/>
-      <c r="B171" s="5"/>
-      <c r="C171" s="13"/>
-      <c r="D171" s="5"/>
-      <c r="E171" s="14"/>
-      <c r="F171" s="11"/>
+      <c r="A171" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B171" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C171" s="13">
+        <v>47805</v>
+      </c>
+      <c r="D171" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E171" s="14">
+        <v>40</v>
+      </c>
+      <c r="F171" s="11">
+        <v>1045.16</v>
+      </c>
       <c r="G171" s="5"/>
       <c r="H171" s="11"/>
       <c r="I171" s="11"/>
@@ -4565,12 +5912,24 @@
       <c r="L171" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="14.25">
-      <c r="A172" s="5"/>
-      <c r="B172" s="5"/>
-      <c r="C172" s="13"/>
-      <c r="D172" s="5"/>
-      <c r="E172" s="14"/>
-      <c r="F172" s="11"/>
+      <c r="A172" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C172" s="13">
+        <v>48899</v>
+      </c>
+      <c r="D172" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E172" s="14">
+        <v>40</v>
+      </c>
+      <c r="F172" s="11">
+        <v>1056.92</v>
+      </c>
       <c r="G172" s="5"/>
       <c r="H172" s="11"/>
       <c r="I172" s="11"/>
@@ -4579,12 +5938,24 @@
       <c r="L172" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="14.25">
-      <c r="A173" s="5"/>
-      <c r="B173" s="5"/>
-      <c r="C173" s="13"/>
-      <c r="D173" s="5"/>
-      <c r="E173" s="14"/>
-      <c r="F173" s="11"/>
+      <c r="A173" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B173" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C173" s="13">
+        <v>46553</v>
+      </c>
+      <c r="D173" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E173" s="14">
+        <v>40</v>
+      </c>
+      <c r="F173" s="11">
+        <v>1316.49</v>
+      </c>
       <c r="G173" s="5"/>
       <c r="H173" s="11"/>
       <c r="I173" s="11"/>
@@ -4593,12 +5964,24 @@
       <c r="L173" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="14.25">
-      <c r="A174" s="5"/>
-      <c r="B174" s="5"/>
-      <c r="C174" s="13"/>
-      <c r="D174" s="5"/>
-      <c r="E174" s="14"/>
-      <c r="F174" s="11"/>
+      <c r="A174" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C174" s="13">
+        <v>47805</v>
+      </c>
+      <c r="D174" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E174" s="14">
+        <v>40</v>
+      </c>
+      <c r="F174" s="11">
+        <v>1251.44</v>
+      </c>
       <c r="G174" s="5"/>
       <c r="H174" s="11"/>
       <c r="I174" s="11"/>
@@ -4607,12 +5990,24 @@
       <c r="L174" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="14.25">
-      <c r="A175" s="5"/>
-      <c r="B175" s="5"/>
-      <c r="C175" s="13"/>
-      <c r="D175" s="5"/>
-      <c r="E175" s="14"/>
-      <c r="F175" s="11"/>
+      <c r="A175" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B175" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C175" s="13">
+        <v>48351</v>
+      </c>
+      <c r="D175" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E175" s="14">
+        <v>40</v>
+      </c>
+      <c r="F175" s="11">
+        <v>1095.55</v>
+      </c>
       <c r="G175" s="5"/>
       <c r="H175" s="11"/>
       <c r="I175" s="11"/>
@@ -4621,12 +6016,24 @@
       <c r="L175" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="14.25">
-      <c r="A176" s="5"/>
-      <c r="B176" s="5"/>
-      <c r="C176" s="13"/>
-      <c r="D176" s="5"/>
-      <c r="E176" s="14"/>
-      <c r="F176" s="11"/>
+      <c r="A176" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C176" s="13">
+        <v>50175</v>
+      </c>
+      <c r="D176" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E176" s="14">
+        <v>40</v>
+      </c>
+      <c r="F176" s="11">
+        <v>1111.79</v>
+      </c>
       <c r="G176" s="5"/>
       <c r="H176" s="11"/>
       <c r="I176" s="11"/>
@@ -4635,12 +6042,24 @@
       <c r="L176" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="14.25">
-      <c r="A177" s="5"/>
-      <c r="B177" s="5"/>
-      <c r="C177" s="13"/>
-      <c r="D177" s="5"/>
-      <c r="E177" s="14"/>
-      <c r="F177" s="11"/>
+      <c r="A177" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B177" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C177" s="13">
+        <v>46615</v>
+      </c>
+      <c r="D177" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E177" s="14">
+        <v>40</v>
+      </c>
+      <c r="F177" s="11">
+        <v>1130.92</v>
+      </c>
       <c r="G177" s="5"/>
       <c r="H177" s="11"/>
       <c r="I177" s="11"/>
@@ -4649,12 +6068,24 @@
       <c r="L177" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="14.25">
-      <c r="A178" s="5"/>
-      <c r="B178" s="5"/>
-      <c r="C178" s="13"/>
-      <c r="D178" s="5"/>
-      <c r="E178" s="14"/>
-      <c r="F178" s="11"/>
+      <c r="A178" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C178" s="13">
+        <v>46615</v>
+      </c>
+      <c r="D178" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="E178" s="14">
+        <v>40</v>
+      </c>
+      <c r="F178" s="11">
+        <v>1037.23</v>
+      </c>
       <c r="G178" s="5"/>
       <c r="H178" s="11"/>
       <c r="I178" s="11"/>
@@ -4663,12 +6094,24 @@
       <c r="L178" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="14.25">
-      <c r="A179" s="5"/>
-      <c r="B179" s="5"/>
-      <c r="C179" s="13"/>
-      <c r="D179" s="5"/>
-      <c r="E179" s="14"/>
-      <c r="F179" s="11"/>
+      <c r="A179" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B179" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C179" s="13">
+        <v>47164</v>
+      </c>
+      <c r="D179" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="E179" s="14">
+        <v>40</v>
+      </c>
+      <c r="F179" s="11">
+        <v>1018.77</v>
+      </c>
       <c r="G179" s="5"/>
       <c r="H179" s="11"/>
       <c r="I179" s="11"/>
@@ -4677,12 +6120,24 @@
       <c r="L179" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="14.25">
-      <c r="A180" s="5"/>
-      <c r="B180" s="5"/>
-      <c r="C180" s="13"/>
-      <c r="D180" s="5"/>
-      <c r="E180" s="14"/>
-      <c r="F180" s="11"/>
+      <c r="A180" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C180" s="13">
+        <v>47896</v>
+      </c>
+      <c r="D180" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="E180" s="14">
+        <v>40</v>
+      </c>
+      <c r="F180" s="11">
+        <v>1022.02</v>
+      </c>
       <c r="G180" s="5"/>
       <c r="H180" s="11"/>
       <c r="I180" s="11"/>
@@ -4691,12 +6146,24 @@
       <c r="L180" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="14.25">
-      <c r="A181" s="5"/>
-      <c r="B181" s="5"/>
-      <c r="C181" s="13"/>
-      <c r="D181" s="5"/>
-      <c r="E181" s="14"/>
-      <c r="F181" s="11"/>
+      <c r="A181" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C181" s="13">
+        <v>47896</v>
+      </c>
+      <c r="D181" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="E181" s="14">
+        <v>40</v>
+      </c>
+      <c r="F181" s="11">
+        <v>992.53</v>
+      </c>
       <c r="G181" s="5"/>
       <c r="H181" s="11"/>
       <c r="I181" s="11"/>
@@ -4705,12 +6172,24 @@
       <c r="L181" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="14.25">
-      <c r="A182" s="5"/>
-      <c r="B182" s="5"/>
-      <c r="C182" s="13"/>
-      <c r="D182" s="5"/>
-      <c r="E182" s="14"/>
-      <c r="F182" s="11"/>
+      <c r="A182" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C182" s="13">
+        <v>46310</v>
+      </c>
+      <c r="D182" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E182" s="14">
+        <v>40</v>
+      </c>
+      <c r="F182" s="11">
+        <v>1197.21</v>
+      </c>
       <c r="G182" s="5"/>
       <c r="H182" s="11"/>
       <c r="I182" s="11"/>
@@ -4719,12 +6198,24 @@
       <c r="L182" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="14.25">
-      <c r="A183" s="5"/>
-      <c r="B183" s="5"/>
-      <c r="C183" s="13"/>
-      <c r="D183" s="5"/>
-      <c r="E183" s="14"/>
-      <c r="F183" s="11"/>
+      <c r="A183" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C183" s="13">
+        <v>48867</v>
+      </c>
+      <c r="D183" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="E183" s="14">
+        <v>40</v>
+      </c>
+      <c r="F183" s="11">
+        <v>1139.85</v>
+      </c>
       <c r="G183" s="5"/>
       <c r="H183" s="11"/>
       <c r="I183" s="11"/>
@@ -4733,12 +6224,24 @@
       <c r="L183" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="14.25">
-      <c r="A184" s="5"/>
-      <c r="B184" s="5"/>
-      <c r="C184" s="13"/>
-      <c r="D184" s="5"/>
-      <c r="E184" s="14"/>
-      <c r="F184" s="11"/>
+      <c r="A184" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C184" s="13">
+        <v>52763</v>
+      </c>
+      <c r="D184" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="E184" s="14">
+        <v>40</v>
+      </c>
+      <c r="F184" s="11">
+        <v>1205.98</v>
+      </c>
       <c r="G184" s="5"/>
       <c r="H184" s="11"/>
       <c r="I184" s="11"/>
@@ -4747,12 +6250,24 @@
       <c r="L184" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="14.25">
-      <c r="A185" s="5"/>
-      <c r="B185" s="5"/>
-      <c r="C185" s="13"/>
-      <c r="D185" s="5"/>
-      <c r="E185" s="14"/>
-      <c r="F185" s="11"/>
+      <c r="A185" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C185" s="13">
+        <v>47192</v>
+      </c>
+      <c r="D185" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E185" s="14">
+        <v>40</v>
+      </c>
+      <c r="F185" s="11">
+        <v>1290.04</v>
+      </c>
       <c r="G185" s="5"/>
       <c r="H185" s="11"/>
       <c r="I185" s="11"/>
@@ -4761,12 +6276,24 @@
       <c r="L185" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="14.25">
-      <c r="A186" s="5"/>
-      <c r="B186" s="5"/>
-      <c r="C186" s="13"/>
-      <c r="D186" s="5"/>
-      <c r="E186" s="14"/>
-      <c r="F186" s="11"/>
+      <c r="A186" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B186" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C186" s="13">
+        <v>46645</v>
+      </c>
+      <c r="D186" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E186" s="14">
+        <v>40</v>
+      </c>
+      <c r="F186" s="11">
+        <v>1240.87</v>
+      </c>
       <c r="G186" s="5"/>
       <c r="H186" s="11"/>
       <c r="I186" s="11"/>
@@ -4775,12 +6302,24 @@
       <c r="L186" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="14.25">
-      <c r="A187" s="5"/>
-      <c r="B187" s="5"/>
-      <c r="C187" s="13"/>
-      <c r="D187" s="5"/>
-      <c r="E187" s="14"/>
-      <c r="F187" s="11"/>
+      <c r="A187" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C187" s="13">
+        <v>46827</v>
+      </c>
+      <c r="D187" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="E187" s="14">
+        <v>35</v>
+      </c>
+      <c r="F187" s="11">
+        <v>1217.96</v>
+      </c>
       <c r="G187" s="5"/>
       <c r="H187" s="11"/>
       <c r="I187" s="11"/>
@@ -4789,12 +6328,24 @@
       <c r="L187" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="14.25">
-      <c r="A188" s="5"/>
-      <c r="B188" s="5"/>
-      <c r="C188" s="13"/>
-      <c r="D188" s="5"/>
-      <c r="E188" s="14"/>
-      <c r="F188" s="11"/>
+      <c r="A188" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C188" s="13">
+        <v>47192</v>
+      </c>
+      <c r="D188" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="E188" s="14">
+        <v>40</v>
+      </c>
+      <c r="F188" s="11">
+        <v>1187.1</v>
+      </c>
       <c r="G188" s="5"/>
       <c r="H188" s="11"/>
       <c r="I188" s="11"/>
@@ -4803,12 +6354,24 @@
       <c r="L188" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="14.25">
-      <c r="A189" s="5"/>
-      <c r="B189" s="5"/>
-      <c r="C189" s="13"/>
-      <c r="D189" s="5"/>
-      <c r="E189" s="14"/>
-      <c r="F189" s="11"/>
+      <c r="A189" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C189" s="13">
+        <v>47102</v>
+      </c>
+      <c r="D189" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="E189" s="14">
+        <v>35</v>
+      </c>
+      <c r="F189" s="11">
+        <v>1248.9</v>
+      </c>
       <c r="G189" s="5"/>
       <c r="H189" s="11"/>
       <c r="I189" s="11"/>
@@ -4817,12 +6380,24 @@
       <c r="L189" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="14.25">
-      <c r="A190" s="5"/>
-      <c r="B190" s="5"/>
-      <c r="C190" s="13"/>
-      <c r="D190" s="5"/>
-      <c r="E190" s="14"/>
-      <c r="F190" s="11"/>
+      <c r="A190" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C190" s="13">
+        <v>46188</v>
+      </c>
+      <c r="D190" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E190" s="14">
+        <v>40</v>
+      </c>
+      <c r="F190" s="11">
+        <v>1336.7</v>
+      </c>
       <c r="G190" s="5"/>
       <c r="H190" s="11"/>
       <c r="I190" s="11"/>
@@ -4831,12 +6406,24 @@
       <c r="L190" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="14.25">
-      <c r="A191" s="5"/>
-      <c r="B191" s="5"/>
-      <c r="C191" s="13"/>
-      <c r="D191" s="5"/>
-      <c r="E191" s="14"/>
-      <c r="F191" s="11"/>
+      <c r="A191" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B191" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C191" s="13">
+        <v>48990</v>
+      </c>
+      <c r="D191" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="E191" s="14">
+        <v>35</v>
+      </c>
+      <c r="F191" s="11">
+        <v>1021.55</v>
+      </c>
       <c r="G191" s="5"/>
       <c r="H191" s="11"/>
       <c r="I191" s="11"/>
@@ -4845,12 +6432,24 @@
       <c r="L191" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="14.25">
-      <c r="A192" s="5"/>
-      <c r="B192" s="5"/>
-      <c r="C192" s="13"/>
-      <c r="D192" s="5"/>
-      <c r="E192" s="14"/>
-      <c r="F192" s="11"/>
+      <c r="A192" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C192" s="13">
+        <v>48014</v>
+      </c>
+      <c r="D192" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="E192" s="14">
+        <v>40</v>
+      </c>
+      <c r="F192" s="11">
+        <v>1048.65</v>
+      </c>
       <c r="G192" s="5"/>
       <c r="H192" s="11"/>
       <c r="I192" s="11"/>
@@ -4859,12 +6458,24 @@
       <c r="L192" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="14.25">
-      <c r="A193" s="5"/>
-      <c r="B193" s="5"/>
-      <c r="C193" s="13"/>
-      <c r="D193" s="5"/>
-      <c r="E193" s="14"/>
-      <c r="F193" s="11"/>
+      <c r="A193" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B193" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C193" s="13">
+        <v>47863</v>
+      </c>
+      <c r="D193" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E193" s="14">
+        <v>35</v>
+      </c>
+      <c r="F193" s="11">
+        <v>1163.37</v>
+      </c>
       <c r="G193" s="5"/>
       <c r="H193" s="11"/>
       <c r="I193" s="11"/>
@@ -4873,12 +6484,24 @@
       <c r="L193" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="14.25">
-      <c r="A194" s="5"/>
-      <c r="B194" s="5"/>
-      <c r="C194" s="13"/>
-      <c r="D194" s="5"/>
-      <c r="E194" s="14"/>
-      <c r="F194" s="11"/>
+      <c r="A194" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C194" s="13">
+        <v>46949</v>
+      </c>
+      <c r="D194" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E194" s="14">
+        <v>40</v>
+      </c>
+      <c r="F194" s="11">
+        <v>1183.48</v>
+      </c>
       <c r="G194" s="5"/>
       <c r="H194" s="11"/>
       <c r="I194" s="11"/>
@@ -4887,12 +6510,24 @@
       <c r="L194" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="14.25">
-      <c r="A195" s="5"/>
-      <c r="B195" s="5"/>
-      <c r="C195" s="13"/>
-      <c r="D195" s="5"/>
-      <c r="E195" s="14"/>
-      <c r="F195" s="11"/>
+      <c r="A195" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B195" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C195" s="13">
+        <v>48014</v>
+      </c>
+      <c r="D195" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E195" s="14">
+        <v>35</v>
+      </c>
+      <c r="F195" s="11">
+        <v>1153.03</v>
+      </c>
       <c r="G195" s="5"/>
       <c r="H195" s="11"/>
       <c r="I195" s="11"/>
@@ -4901,12 +6536,24 @@
       <c r="L195" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="14.25">
-      <c r="A196" s="5"/>
-      <c r="B196" s="5"/>
-      <c r="C196" s="13"/>
-      <c r="D196" s="5"/>
-      <c r="E196" s="14"/>
-      <c r="F196" s="11"/>
+      <c r="A196" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C196" s="13">
+        <v>49049</v>
+      </c>
+      <c r="D196" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E196" s="14">
+        <v>40</v>
+      </c>
+      <c r="F196" s="11">
+        <v>1042.18</v>
+      </c>
       <c r="G196" s="5"/>
       <c r="H196" s="11"/>
       <c r="I196" s="11"/>
@@ -4915,12 +6562,24 @@
       <c r="L196" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="14.25">
-      <c r="A197" s="5"/>
-      <c r="B197" s="5"/>
-      <c r="C197" s="13"/>
-      <c r="D197" s="5"/>
-      <c r="E197" s="14"/>
-      <c r="F197" s="11"/>
+      <c r="A197" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B197" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C197" s="13">
+        <v>50601</v>
+      </c>
+      <c r="D197" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E197" s="14">
+        <v>35</v>
+      </c>
+      <c r="F197" s="11">
+        <v>1074.98</v>
+      </c>
       <c r="G197" s="5"/>
       <c r="H197" s="11"/>
       <c r="I197" s="11"/>
@@ -4929,12 +6588,24 @@
       <c r="L197" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="14.25">
-      <c r="A198" s="5"/>
-      <c r="B198" s="5"/>
-      <c r="C198" s="13"/>
-      <c r="D198" s="5"/>
-      <c r="E198" s="14"/>
-      <c r="F198" s="11"/>
+      <c r="A198" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C198" s="13">
+        <v>48410</v>
+      </c>
+      <c r="D198" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="E198" s="14">
+        <v>40</v>
+      </c>
+      <c r="F198" s="11">
+        <v>1121.61</v>
+      </c>
       <c r="G198" s="5"/>
       <c r="H198" s="11"/>
       <c r="I198" s="11"/>
@@ -4943,12 +6614,24 @@
       <c r="L198" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="14.25">
-      <c r="A199" s="5"/>
-      <c r="B199" s="5"/>
-      <c r="C199" s="13"/>
-      <c r="D199" s="5"/>
-      <c r="E199" s="14"/>
-      <c r="F199" s="11"/>
+      <c r="A199" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C199" s="13">
+        <v>49871</v>
+      </c>
+      <c r="D199" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="E199" s="14">
+        <v>35</v>
+      </c>
+      <c r="F199" s="11">
+        <v>1066.32</v>
+      </c>
       <c r="G199" s="5"/>
       <c r="H199" s="11"/>
       <c r="I199" s="11"/>
@@ -4957,12 +6640,24 @@
       <c r="L199" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="14.25">
-      <c r="A200" s="5"/>
-      <c r="B200" s="5"/>
-      <c r="C200" s="13"/>
-      <c r="D200" s="5"/>
-      <c r="E200" s="14"/>
-      <c r="F200" s="11"/>
+      <c r="A200" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C200" s="13">
+        <v>50236</v>
+      </c>
+      <c r="D200" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E200" s="14">
+        <v>40</v>
+      </c>
+      <c r="F200" s="11">
+        <v>1134.43</v>
+      </c>
       <c r="G200" s="5"/>
       <c r="H200" s="11"/>
       <c r="I200" s="11"/>
@@ -4971,12 +6666,24 @@
       <c r="L200" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="14.25">
-      <c r="A201" s="5"/>
-      <c r="B201" s="5"/>
-      <c r="C201" s="13"/>
-      <c r="D201" s="5"/>
-      <c r="E201" s="14"/>
-      <c r="F201" s="11"/>
+      <c r="A201" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B201" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C201" s="13">
+        <v>49110</v>
+      </c>
+      <c r="D201" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="E201" s="14">
+        <v>35</v>
+      </c>
+      <c r="F201" s="11">
+        <v>1066.81</v>
+      </c>
       <c r="G201" s="5"/>
       <c r="H201" s="11"/>
       <c r="I201" s="11"/>
@@ -4985,12 +6692,24 @@
       <c r="L201" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="14.25">
-      <c r="A202" s="5"/>
-      <c r="B202" s="5"/>
-      <c r="C202" s="13"/>
-      <c r="D202" s="5"/>
-      <c r="E202" s="14"/>
-      <c r="F202" s="11"/>
+      <c r="A202" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B202" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C202" s="13">
+        <v>50936</v>
+      </c>
+      <c r="D202" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="E202" s="14">
+        <v>40</v>
+      </c>
+      <c r="F202" s="11">
+        <v>1081.16</v>
+      </c>
       <c r="G202" s="5"/>
       <c r="H202" s="11"/>
       <c r="I202" s="11"/>
@@ -4999,12 +6718,24 @@
       <c r="L202" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="14.25">
-      <c r="A203" s="5"/>
-      <c r="B203" s="5"/>
-      <c r="C203" s="13"/>
-      <c r="D203" s="5"/>
-      <c r="E203" s="14"/>
-      <c r="F203" s="11"/>
+      <c r="A203" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B203" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C203" s="13">
+        <v>47953</v>
+      </c>
+      <c r="D203" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E203" s="14">
+        <v>35</v>
+      </c>
+      <c r="F203" s="11">
+        <v>1179.28</v>
+      </c>
       <c r="G203" s="5"/>
       <c r="H203" s="11"/>
       <c r="I203" s="11"/>
@@ -5013,12 +6744,24 @@
       <c r="L203" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="14.25">
-      <c r="A204" s="5"/>
-      <c r="B204" s="5"/>
-      <c r="C204" s="13"/>
-      <c r="D204" s="5"/>
-      <c r="E204" s="14"/>
-      <c r="F204" s="11"/>
+      <c r="A204" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C204" s="13">
+        <v>47953</v>
+      </c>
+      <c r="D204" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="E204" s="14">
+        <v>40</v>
+      </c>
+      <c r="F204" s="11">
+        <v>1040.64</v>
+      </c>
       <c r="G204" s="5"/>
       <c r="H204" s="11"/>
       <c r="I204" s="11"/>
@@ -5027,12 +6770,24 @@
       <c r="L204" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="14.25">
-      <c r="A205" s="5"/>
-      <c r="B205" s="5"/>
-      <c r="C205" s="13"/>
-      <c r="D205" s="5"/>
-      <c r="E205" s="14"/>
-      <c r="F205" s="11"/>
+      <c r="A205" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B205" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C205" s="13">
+        <v>47649</v>
+      </c>
+      <c r="D205" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="E205" s="14">
+        <v>35</v>
+      </c>
+      <c r="F205" s="11">
+        <v>1061.49</v>
+      </c>
       <c r="G205" s="5"/>
       <c r="H205" s="11"/>
       <c r="I205" s="11"/>
@@ -5041,12 +6796,24 @@
       <c r="L205" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="14.25">
-      <c r="A206" s="5"/>
-      <c r="B206" s="5"/>
-      <c r="C206" s="13"/>
-      <c r="D206" s="5"/>
-      <c r="E206" s="14"/>
-      <c r="F206" s="11"/>
+      <c r="A206" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C206" s="13">
+        <v>47649</v>
+      </c>
+      <c r="D206" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="E206" s="14">
+        <v>40</v>
+      </c>
+      <c r="F206" s="11">
+        <v>1074.04</v>
+      </c>
       <c r="G206" s="5"/>
       <c r="H206" s="11"/>
       <c r="I206" s="11"/>
@@ -5055,12 +6822,24 @@
       <c r="L206" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="14.25">
-      <c r="A207" s="5"/>
-      <c r="B207" s="5"/>
-      <c r="C207" s="13"/>
-      <c r="D207" s="5"/>
-      <c r="E207" s="14"/>
-      <c r="F207" s="11"/>
+      <c r="A207" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B207" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C207" s="13">
+        <v>46157</v>
+      </c>
+      <c r="D207" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E207" s="14">
+        <v>35</v>
+      </c>
+      <c r="F207" s="11">
+        <v>1320.22</v>
+      </c>
       <c r="G207" s="5"/>
       <c r="H207" s="11"/>
       <c r="I207" s="11"/>
@@ -5069,12 +6848,24 @@
       <c r="L207" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="14.25">
-      <c r="A208" s="5"/>
-      <c r="B208" s="5"/>
-      <c r="C208" s="13"/>
-      <c r="D208" s="5"/>
-      <c r="E208" s="14"/>
-      <c r="F208" s="11"/>
+      <c r="A208" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B208" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C208" s="13">
+        <v>46127</v>
+      </c>
+      <c r="D208" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E208" s="14">
+        <v>40</v>
+      </c>
+      <c r="F208" s="11">
+        <v>1346.48</v>
+      </c>
       <c r="G208" s="5"/>
       <c r="H208" s="11"/>
       <c r="I208" s="11"/>
@@ -5083,12 +6874,24 @@
       <c r="L208" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="14.25">
-      <c r="A209" s="5"/>
-      <c r="B209" s="5"/>
-      <c r="C209" s="13"/>
-      <c r="D209" s="5"/>
-      <c r="E209" s="14"/>
-      <c r="F209" s="11"/>
+      <c r="A209" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B209" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C209" s="13">
+        <v>45573</v>
+      </c>
+      <c r="D209" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E209" s="14">
+        <v>1</v>
+      </c>
+      <c r="F209" s="11">
+        <v>10</v>
+      </c>
       <c r="G209" s="5"/>
       <c r="H209" s="11"/>
       <c r="I209" s="11"/>

</xml_diff>